<commit_message>
Más tratamiento de datos
Incluido el one-hot
</commit_message>
<xml_diff>
--- a/Métricas.xlsx
+++ b/Métricas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Documents\GitHub\UniversityHack-2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FFB2F9-D940-4B0A-A986-380473E19910}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC516B0-F3D5-44B2-9F30-B5F326687A26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t>concensoV1.0</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>0.56</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>concensoV1.1</t>
+  </si>
+  <si>
+    <t>concensoV1.2</t>
   </si>
 </sst>
 </file>
@@ -385,27 +394,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.88671875" customWidth="1"/>
     <col min="2" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -413,10 +426,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -424,10 +440,13 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -435,10 +454,13 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -446,10 +468,13 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
     </row>
   </sheetData>

</xml_diff>